<commit_message>
Integrating way to update payment history
</commit_message>
<xml_diff>
--- a/server/data/data.xlsx
+++ b/server/data/data.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -457,14 +457,29 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="str">
+        <v>kennedy.ads@gmail.com</v>
+      </c>
+      <c r="C4">
+        <v>710943451</v>
+      </c>
+      <c r="D4" t="str">
+        <v>$2b$10$QErIzwxCF2DMPC8bd2TPou7uEnEm.bsZ6lahX1mAufcA5SF.hnaP2</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>